<commit_message>
New SCAS models, read the docs changes
</commit_message>
<xml_diff>
--- a/Benchmarking/Li_Zhang/PySulfSat_Input.xlsx
+++ b/Benchmarking/Li_Zhang/PySulfSat_Input.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Berkeley_NEW\PySulfSat\PySulfSat_Structure\Benchmarking\Li_Zhang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6DCEEA-4293-445D-991F-8144419D7A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E02FC2A-962F-41A9-9200-CEA910EEC7AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{94C6C78D-22F8-4936-9B41-A7B46E91FA87}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15510" xr2:uid="{94C6C78D-22F8-4936-9B41-A7B46E91FA87}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -257,9 +257,6 @@
     <t>Fe/(Fe+Cu+Ni)</t>
   </si>
   <si>
-    <t>H2O(wt%)</t>
-  </si>
-  <si>
     <t>S total cal</t>
   </si>
   <si>
@@ -339,6 +336,9 @@
   </si>
   <si>
     <t>HS cal2</t>
+  </si>
+  <si>
+    <t>H2O_Liq</t>
   </si>
 </sst>
 </file>
@@ -693,7 +693,7 @@
   <dimension ref="A1:AV69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -724,7 +724,7 @@
         <v>65</v>
       </c>
       <c r="I1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J1" t="s">
         <v>66</v>
@@ -748,88 +748,88 @@
         <v>72</v>
       </c>
       <c r="Q1" t="s">
+        <v>100</v>
+      </c>
+      <c r="R1" t="s">
         <v>73</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>74</v>
-      </c>
-      <c r="S1" t="s">
-        <v>75</v>
       </c>
       <c r="T1" t="s">
         <v>62</v>
       </c>
       <c r="U1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="V1" t="s">
+        <v>77</v>
+      </c>
+      <c r="W1" t="s">
         <v>78</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>79</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>80</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>81</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>82</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>83</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>84</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>85</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>86</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>87</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>88</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>89</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>90</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>91</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>92</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>93</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>94</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>95</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>96</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AT1" t="s">
         <v>97</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>98</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>99</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.35">

</xml_diff>